<commit_message>
Added new test case to analysis stock
</commit_message>
<xml_diff>
--- a/src/test/resources/OtherData/StockName.xlsx
+++ b/src/test/resources/OtherData/StockName.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>StockName</t>
   </si>
@@ -76,6 +76,93 @@
   </si>
   <si>
     <t>mphasis share price</t>
+  </si>
+  <si>
+    <t>Asian Pain Share Price</t>
+  </si>
+  <si>
+    <t>wipro share price</t>
+  </si>
+  <si>
+    <t>lti mindtree share price</t>
+  </si>
+  <si>
+    <t>sonata software share price</t>
+  </si>
+  <si>
+    <t>Honeywell share price</t>
+  </si>
+  <si>
+    <t>20/12/2022</t>
+  </si>
+  <si>
+    <t>−34.70</t>
+  </si>
+  <si>
+    <t>−147.85</t>
+  </si>
+  <si>
+    <t>+0.080</t>
+  </si>
+  <si>
+    <t>−14.90</t>
+  </si>
+  <si>
+    <t>−58.55</t>
+  </si>
+  <si>
+    <t>−4.45</t>
+  </si>
+  <si>
+    <t>−0.80</t>
+  </si>
+  <si>
+    <t>+11.95</t>
+  </si>
+  <si>
+    <t>−3.05</t>
+  </si>
+  <si>
+    <t>−7.90</t>
+  </si>
+  <si>
+    <t>−1.40</t>
+  </si>
+  <si>
+    <t>−9.65</t>
+  </si>
+  <si>
+    <t>−30.10</t>
+  </si>
+  <si>
+    <t>−8.50</t>
+  </si>
+  <si>
+    <t>−7.25</t>
+  </si>
+  <si>
+    <t>−57.85</t>
+  </si>
+  <si>
+    <t>−14.95</t>
+  </si>
+  <si>
+    <t>+16.15</t>
+  </si>
+  <si>
+    <t>−14.05</t>
+  </si>
+  <si>
+    <t>−2.45</t>
+  </si>
+  <si>
+    <t>−36.05</t>
+  </si>
+  <si>
+    <t>−14.65</t>
+  </si>
+  <si>
+    <t>−0.33</t>
   </si>
 </sst>
 </file>
@@ -400,110 +487,208 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A19"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="43.140625" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>